<commit_message>
added add/del column color coding to create_comparison_excel() and updated README
</commit_message>
<xml_diff>
--- a/inst/extdata/comparison_report.xlsx
+++ b/inst/extdata/comparison_report.xlsx
@@ -21,13 +21,13 @@
     <sheet name="df2" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'df2'!$A$1:$K$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'df2'!$A$1:$L$9</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t xml:space="preserve">Columns</t>
   </si>
@@ -41,6 +41,12 @@
     <t xml:space="preserve">Total</t>
   </si>
   <si>
+    <t xml:space="preserve">Added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted</t>
+  </si>
+  <si>
     <t xml:space="preserve">Changed</t>
   </si>
   <si>
@@ -50,12 +56,6 @@
     <t xml:space="preserve">Rows</t>
   </si>
   <si>
-    <t xml:space="preserve">Added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deleted</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unchanged</t>
   </si>
   <si>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">Changes</t>
   </si>
   <si>
-    <t xml:space="preserve">Mismatched class</t>
+    <t xml:space="preserve">Classes match</t>
   </si>
   <si>
     <t xml:space="preserve">df1 class</t>
@@ -137,6 +137,12 @@
     <t xml:space="preserve">dec_diff</t>
   </si>
   <si>
+    <t xml:space="preserve">extra1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra2</t>
+  </si>
+  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
@@ -230,9 +236,6 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">matched</t>
-  </si>
-  <si>
     <t xml:space="preserve">exact dup cnt.df1</t>
   </si>
   <si>
@@ -291,6 +294,18 @@
   </si>
   <si>
     <t xml:space="preserve">dec_diff.df2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra1.df1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra1.df2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra2.df1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra2.df2</t>
   </si>
   <si>
     <t xml:space="preserve">exact duplicate</t>
@@ -403,7 +418,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -713,10 +742,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -724,61 +753,61 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>2</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -786,40 +815,36 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0</v>
@@ -827,12 +852,34 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="n">
+      <c r="B16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -867,11 +914,13 @@
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -880,10 +929,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -912,6 +961,12 @@
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -921,10 +976,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>2</v>
@@ -933,7 +988,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>5</v>
@@ -942,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="n">
@@ -954,6 +1009,10 @@
       <c r="N2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -963,10 +1022,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>2</v>
@@ -975,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>5</v>
@@ -984,10 +1043,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="n">
@@ -996,9 +1055,13 @@
       <c r="N3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="O3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N3"/>
+  <autoFilter ref="A1:P3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -1028,11 +1091,13 @@
     <col min="11" max="11" width="15.71" hidden="0" customWidth="1"/>
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -1041,7 +1106,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
@@ -1070,6 +1135,12 @@
       <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -1080,13 +1151,13 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>5</v>
@@ -1095,10 +1166,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="n">
@@ -1107,9 +1178,13 @@
       <c r="M2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M2"/>
+  <autoFilter ref="A1:O2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -1137,6 +1212,7 @@
     <col min="9" max="9" width="15.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="15.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="15.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1173,19 +1249,22 @@
       <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
@@ -1204,13 +1283,16 @@
       <c r="K2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2</v>
@@ -1231,17 +1313,20 @@
       <c r="K3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>2</v>
@@ -1261,6 +1346,9 @@
       </c>
       <c r="K4" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -1268,13 +1356,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>3</v>
@@ -1293,19 +1381,22 @@
       <c r="K5" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>5</v>
@@ -1326,19 +1417,22 @@
       <c r="K6" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L6" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>5</v>
@@ -1359,19 +1453,22 @@
       <c r="K7" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L7" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>5</v>
@@ -1392,19 +1489,22 @@
       <c r="K8" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L8" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>5</v>
@@ -1425,6 +1525,9 @@
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L9" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1435,7 +1538,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>5</v>
@@ -1455,6 +1558,9 @@
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -1462,13 +1568,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>5</v>
@@ -1489,9 +1595,12 @@
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L11" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K11"/>
+  <autoFilter ref="A1:L11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -1519,6 +1628,7 @@
     <col min="9" max="9" width="15.71" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="15.71" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="15.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1555,19 +1665,22 @@
       <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
@@ -1577,7 +1690,7 @@
         <v>44927</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="n">
@@ -1586,19 +1699,22 @@
       <c r="K2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
@@ -1608,7 +1724,7 @@
         <v>44927</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="n">
@@ -1617,19 +1733,22 @@
       <c r="K3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>1</v>
@@ -1639,7 +1758,7 @@
         <v>44927</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="n">
@@ -1648,13 +1767,16 @@
       <c r="K4" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
@@ -1666,7 +1788,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="n">
@@ -1675,17 +1797,20 @@
       <c r="K5" s="2" t="n">
         <v>1.0001</v>
       </c>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>2</v>
@@ -1697,7 +1822,7 @@
         <v>44929</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="n">
@@ -1706,19 +1831,22 @@
       <c r="K6" s="2" t="n">
         <v>1.00001</v>
       </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>3</v>
@@ -1728,7 +1856,7 @@
         <v>44930</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="n">
@@ -1737,19 +1865,22 @@
       <c r="K7" s="2" t="n">
         <v>1.000001</v>
       </c>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>6</v>
@@ -1761,7 +1892,7 @@
         <v>44932</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="n">
@@ -1769,6 +1900,9 @@
       </c>
       <c r="K8" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -1776,13 +1910,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>5</v>
@@ -1794,7 +1928,7 @@
         <v>44931</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="n">
@@ -1803,9 +1937,12 @@
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L9" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K9"/>
+  <autoFilter ref="A1:L9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -1867,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>21</v>
@@ -1890,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>23</v>
@@ -1913,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>21</v>
@@ -1936,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
@@ -1959,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>27</v>
@@ -1982,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>29</v>
@@ -2005,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>31</v>
@@ -2028,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>21</v>
@@ -2051,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>21</v>
@@ -2074,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
@@ -2097,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
@@ -2106,8 +2243,51 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G12"/>
+  <autoFilter ref="A1:G14"/>
+  <conditionalFormatting sqref="B2:E14">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE", B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -2140,11 +2320,13 @@
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
     <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
     <col min="16" max="16" width="15.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="15.71" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -2153,16 +2335,16 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -2191,6 +2373,12 @@
       <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -2200,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
@@ -2214,17 +2402,17 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3" t="n">
@@ -2233,6 +2421,10 @@
       <c r="P2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -2242,10 +2434,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
@@ -2258,17 +2450,17 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="4" t="n">
@@ -2277,6 +2469,10 @@
       <c r="P3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -2286,10 +2482,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>2</v>
@@ -2306,7 +2502,7 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="3" t="n">
@@ -2315,6 +2511,10 @@
       <c r="P4" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="Q4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -2324,10 +2524,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>2</v>
@@ -2344,7 +2544,7 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="4" t="n">
@@ -2353,6 +2553,10 @@
       <c r="P5" s="4" t="n">
         <v>1.0001</v>
       </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -2362,10 +2566,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>3</v>
@@ -2374,7 +2578,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>2</v>
@@ -2383,10 +2587,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="3" t="n">
@@ -2395,6 +2599,10 @@
       <c r="P6" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="Q6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -2404,10 +2612,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>3</v>
@@ -2416,7 +2624,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>2</v>
@@ -2425,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="4" t="n">
@@ -2437,6 +2645,10 @@
       <c r="P7" s="4" t="n">
         <v>1.00001</v>
       </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -2446,10 +2658,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>4</v>
@@ -2460,17 +2672,17 @@
         <v>4</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="3" t="n">
@@ -2479,6 +2691,10 @@
       <c r="P8" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -2488,10 +2704,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>4</v>
@@ -2502,17 +2718,17 @@
         <v>4</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>3</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="4" t="n">
@@ -2521,6 +2737,10 @@
       <c r="P9" s="2" t="n">
         <v>1.000001</v>
       </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -2530,10 +2750,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2544,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>5</v>
@@ -2553,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="n">
@@ -2565,6 +2785,10 @@
       <c r="P10" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -2574,10 +2798,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -2588,7 +2812,7 @@
         <v>5</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>5</v>
@@ -2597,10 +2821,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="n">
@@ -2609,6 +2833,10 @@
       <c r="P11" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="4"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -2618,10 +2846,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="n">
@@ -2632,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J12" s="3" t="n">
         <v>5</v>
@@ -2641,10 +2869,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="n">
@@ -2653,6 +2881,10 @@
       <c r="P12" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="Q12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
@@ -2663,7 +2895,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -2672,7 +2904,7 @@
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>5</v>
@@ -2681,10 +2913,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="n">
@@ -2693,6 +2925,10 @@
       <c r="P13" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -2702,10 +2938,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2714,7 +2950,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J14" s="4" t="n">
         <v>6</v>
@@ -2723,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="n">
@@ -2735,6 +2971,10 @@
       <c r="P14" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -2744,19 +2984,21 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>7</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="n">
         <v>5</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J15" s="2" t="n">
         <v>5</v>
@@ -2765,10 +3007,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="n">
@@ -2777,9 +3019,61 @@
       <c r="P15" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Q15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P15"/>
+  <autoFilter ref="A1:R16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -2809,88 +3103,76 @@
     <col min="11" max="11" width="15.71" hidden="0" customWidth="1"/>
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M2"/>
+  <autoFilter ref="A1:O1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -2921,11 +3203,12 @@
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -2934,10 +3217,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -2966,6 +3249,9 @@
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -2975,31 +3261,31 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="n">
@@ -3008,9 +3294,12 @@
       <c r="N2" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N2"/>
+  <autoFilter ref="A1:O2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -3041,11 +3330,12 @@
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -3054,10 +3344,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -3086,6 +3376,9 @@
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -3095,17 +3388,17 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="4" t="n">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>6</v>
@@ -3114,10 +3407,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="n">
@@ -3126,9 +3419,12 @@
       <c r="N2" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="O2" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N2"/>
+  <autoFilter ref="A1:O2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -3160,11 +3456,13 @@
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
     <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="15.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -3173,13 +3471,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>24</v>
@@ -3208,6 +3506,12 @@
       <c r="O1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -3217,10 +3521,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
@@ -3230,17 +3534,17 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="3" t="n">
@@ -3249,6 +3553,10 @@
       <c r="O2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="P2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -3258,10 +3566,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>1</v>
@@ -3273,17 +3581,17 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="4" t="n">
@@ -3292,6 +3600,10 @@
       <c r="O3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -3301,10 +3613,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>2</v>
@@ -3320,7 +3632,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="3" t="n">
@@ -3329,6 +3641,10 @@
       <c r="O4" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -3338,10 +3654,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>2</v>
@@ -3357,7 +3673,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="4" t="n">
@@ -3366,6 +3682,10 @@
       <c r="O5" s="4" t="n">
         <v>1.0001</v>
       </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -3375,10 +3695,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>3</v>
@@ -3386,7 +3706,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>2</v>
@@ -3395,10 +3715,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="3" t="n">
@@ -3407,6 +3727,10 @@
       <c r="O6" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="P6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -3416,10 +3740,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>3</v>
@@ -3427,7 +3751,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>2</v>
@@ -3436,10 +3760,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="4" t="n">
@@ -3448,6 +3772,10 @@
       <c r="O7" s="4" t="n">
         <v>1.00001</v>
       </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -3457,10 +3785,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>4</v>
@@ -3470,17 +3798,17 @@
         <v>4</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="3" t="n">
@@ -3489,6 +3817,10 @@
       <c r="O8" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="P8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -3498,10 +3830,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>4</v>
@@ -3511,17 +3843,17 @@
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>3</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="4" t="n">
@@ -3530,9 +3862,107 @@
       <c r="O9" s="2" t="n">
         <v>1.000001</v>
       </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O9"/>
+  <autoFilter ref="A1:Q11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -3573,6 +4003,10 @@
     <col min="22" max="22" width="15.71" hidden="0" customWidth="1"/>
     <col min="23" max="23" width="15.71" hidden="0" customWidth="1"/>
     <col min="24" max="24" width="15.71" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="15.71" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="15.71" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="15.71" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3583,70 +4017,82 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2">
@@ -3654,10 +4100,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>1</v>
@@ -3673,10 +4119,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>1</v>
@@ -3687,16 +4133,16 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -3712,16 +4158,24 @@
       <c r="X2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="Y2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>2</v>
@@ -3747,10 +4201,10 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -3766,16 +4220,24 @@
       <c r="X3" s="4" t="n">
         <v>1.0001</v>
       </c>
+      <c r="Y3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>3</v>
@@ -3785,10 +4247,10 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>2</v>
@@ -3803,16 +4265,16 @@
         <v>0</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -3828,16 +4290,24 @@
       <c r="X4" s="4" t="n">
         <v>1.00001</v>
       </c>
+      <c r="Y4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>4</v>
@@ -3851,10 +4321,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>3</v>
@@ -3865,16 +4335,16 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -3890,9 +4360,91 @@
       <c r="X5" s="2" t="n">
         <v>1.000001</v>
       </c>
+      <c r="Y5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X5"/>
+  <autoFilter ref="A1:AB6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -3923,11 +4475,13 @@
     <col min="12" max="12" width="15.71" hidden="0" customWidth="1"/>
     <col min="13" max="13" width="15.71" hidden="0" customWidth="1"/>
     <col min="14" max="14" width="15.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="15.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -3936,10 +4490,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -3968,6 +4522,12 @@
       <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -3977,31 +4537,31 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="n">
@@ -4010,6 +4570,10 @@
       <c r="N2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="4"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -4019,10 +4583,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>3</v>
@@ -4031,17 +4595,17 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="n">
@@ -4050,9 +4614,13 @@
       <c r="N3" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N3"/>
+  <autoFilter ref="A1:P3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
updated color coding of Excel report
</commit_message>
<xml_diff>
--- a/inst/extdata/comparison_report.xlsx
+++ b/inst/extdata/comparison_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t xml:space="preserve">Summary: df1 and df2 have different records and/or non-unique records</t>
   </si>
@@ -175,12 +175,12 @@
     <t xml:space="preserve">extra2</t>
   </si>
   <si>
+    <t xml:space="preserve">discrepancy</t>
+  </si>
+  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
-    <t xml:space="preserve">discrepancy</t>
-  </si>
-  <si>
     <t xml:space="preserve">change group</t>
   </si>
   <si>
@@ -268,6 +268,18 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
+    <t xml:space="preserve">exact dup cnt.df1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exact dup cnt.df2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID dup cnt.df1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID dup cnt.df2</t>
+  </si>
+  <si>
     <t xml:space="preserve">num.df1</t>
   </si>
   <si>
@@ -332,6 +344,12 @@
   </si>
   <si>
     <t xml:space="preserve">extra2.df2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df1 ID duplicate (not exact duplicate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df1 ID contains `NA`</t>
   </si>
 </sst>
 </file>
@@ -368,13 +386,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF32CD32"/>
       <name val="Calibri"/>
       <b/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF3030"/>
       <name val="Calibri"/>
       <b/>
     </font>
@@ -398,7 +416,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
   </fills>
@@ -428,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,10 +461,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -1351,9 +1378,9 @@
   <cols>
     <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
-    <col min="4" max="4" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
-    <col min="5" max="5" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
+    <col min="3" max="3" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="4" max="4" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="5" max="5" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
     <col min="6" max="6" width="15.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="15.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
@@ -1427,10 +1454,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1</v>
@@ -1460,71 +1487,71 @@
         <v>60</v>
       </c>
       <c r="N2" s="5"/>
-      <c r="O2" s="6" t="n">
+      <c r="O2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="P2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="7"/>
+      <c r="R2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="n">
+      <c r="C3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
+      <c r="J3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="7" t="s">
+      <c r="M3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>2</v>
@@ -1550,65 +1577,65 @@
         <v>60</v>
       </c>
       <c r="N4" s="5"/>
-      <c r="O4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="O4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="7"/>
+      <c r="R4" s="10"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="C5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="7" t="n">
+      <c r="H5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="8" t="n">
         <v>-0.0001</v>
       </c>
-      <c r="P5" s="7" t="n">
+      <c r="P5" s="8" t="n">
         <v>1.0001</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="7" t="s">
+      <c r="Q5" s="9"/>
+      <c r="R5" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>3</v>
@@ -1638,69 +1665,69 @@
         <v>60</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="O6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="7"/>
+      <c r="R6" s="10"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="n">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="J7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="7" t="n">
+      <c r="M7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="8" t="n">
         <v>-0.00001</v>
       </c>
-      <c r="P7" s="7" t="n">
+      <c r="P7" s="8" t="n">
         <v>1.00001</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="7" t="s">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>4</v>
@@ -1730,69 +1757,69 @@
         <v>60</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="6" t="n">
+      <c r="O8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="P8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="Q8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="7"/>
+      <c r="R8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="n">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="7" t="n">
+      <c r="M9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8" t="n">
         <v>-0.000001</v>
       </c>
-      <c r="P9" s="5" t="n">
+      <c r="P9" s="6" t="n">
         <v>1.000001</v>
       </c>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="7" t="s">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1830,17 +1857,17 @@
       <c r="P10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="7"/>
+      <c r="R10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1878,17 +1905,17 @@
       <c r="P11" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="Q11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R11" s="7"/>
+      <c r="R11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="n">
@@ -1901,42 +1928,42 @@
       <c r="G12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="K12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="J12" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6" t="s">
+      <c r="M12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R12" s="7"/>
+      <c r="R12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1970,63 +1997,63 @@
       <c r="P13" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="Q13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="7"/>
+      <c r="R13" s="10"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="n">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="K14" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="L14" s="7" t="s">
+      <c r="K14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="7" t="s">
+      <c r="M14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>7</v>
@@ -2064,56 +2091,56 @@
       <c r="P15" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R15" s="7"/>
+      <c r="R15" s="10"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="n">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="K16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="J16" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="P16" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="7" t="s">
+      <c r="M16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2129,18 +2156,18 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
-      <pane ySplit="1" xSplit="7" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane ySplit="1" xSplit="8" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
-    <col min="4" max="4" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
-    <col min="5" max="5" width="15.71" hidden="0" outlineLevel="1" customWidth="1"/>
-    <col min="6" max="6" width="15.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="3" max="3" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="4" max="4" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="5" max="5" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
+    <col min="6" max="6" width="15.71" hidden="1" outlineLevel="1" customWidth="1"/>
     <col min="7" max="7" width="15.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="15.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="15.71" hidden="0" customWidth="1"/>
@@ -2164,6 +2191,7 @@
     <col min="27" max="27" width="15.71" hidden="0" customWidth="1"/>
     <col min="28" max="28" width="15.71" hidden="0" customWidth="1"/>
     <col min="29" max="29" width="15.71" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2171,703 +2199,737 @@
         <v>51</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5"/>
+      <c r="B2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="5" t="n">
-        <v>1</v>
-      </c>
       <c r="I2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>58</v>
+      <c r="J2" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="5" t="n">
-        <v>1</v>
+      <c r="L2" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="5"/>
+      <c r="N2" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="P2" s="6"/>
       <c r="Q2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>60</v>
+      <c r="R2" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="5"/>
+      <c r="T2" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="U2" s="5"/>
-      <c r="V2" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="V2" s="6"/>
       <c r="W2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" s="5" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="X2" s="8" t="n">
+        <v>0</v>
       </c>
       <c r="Y2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="7" t="s">
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5"/>
+      <c r="B3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="5" t="n">
-        <v>2</v>
-      </c>
       <c r="I3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="N3" s="6"/>
       <c r="O3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="R3" s="6"/>
       <c r="S3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="T3" s="5"/>
+      <c r="T3" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="U3" s="5"/>
-      <c r="V3" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="V3" s="6"/>
       <c r="W3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="8" t="n">
         <v>-0.0001</v>
       </c>
-      <c r="X3" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="Y3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="8" t="n">
         <v>1.0001</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="7" t="s">
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="B4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="6"/>
+      <c r="G4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="5" t="n">
-        <v>2</v>
+      <c r="L4" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="N4" s="5" t="b">
-        <v>0</v>
+      <c r="N4" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="O4" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>65</v>
+      <c r="P4" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>60</v>
+      <c r="R4" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="T4" s="5"/>
+      <c r="T4" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="U4" s="5"/>
-      <c r="V4" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="V4" s="6"/>
       <c r="W4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="8" t="n">
         <v>-0.00001</v>
       </c>
-      <c r="X4" s="6" t="n">
-        <v>1</v>
-      </c>
       <c r="Y4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="8" t="n">
         <v>1.00001</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="AA4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="7" t="s">
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="B5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="6"/>
+      <c r="G5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>4</v>
       </c>
       <c r="I5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>67</v>
+      <c r="J5" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="5" t="n">
-        <v>3</v>
+      <c r="L5" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="N5" s="5"/>
+      <c r="N5" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="P5" s="6"/>
       <c r="Q5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>60</v>
+      <c r="R5" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="T5" s="5"/>
+      <c r="T5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="U5" s="5"/>
-      <c r="V5" s="6" t="n">
-        <v>1</v>
-      </c>
+      <c r="V5" s="6"/>
       <c r="W5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="8" t="n">
         <v>-0.000001</v>
       </c>
-      <c r="X5" s="5" t="n">
-        <v>1</v>
-      </c>
       <c r="Y5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="6" t="n">
         <v>1.000001</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="AA5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="7" t="s">
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="I6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="5" t="s">
+      <c r="L6" s="9"/>
+      <c r="M6" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="9"/>
+      <c r="O6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W6" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="6" t="s">
+      <c r="R6" s="9"/>
+      <c r="S6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T6" s="9"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="8"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="N7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="X7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="6" t="s">
+      <c r="R7" s="9"/>
+      <c r="S7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="9"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
+      <c r="I8" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5" t="s">
+      <c r="L8" s="9"/>
+      <c r="M8" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="6" t="s">
+      <c r="R8" s="9"/>
+      <c r="S8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="6"/>
+      <c r="AB8" s="8"/>
       <c r="AC8" s="7"/>
+      <c r="AD8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5" t="s">
+      <c r="L9" s="9"/>
+      <c r="M9" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="6" t="s">
+      <c r="R9" s="9"/>
+      <c r="S9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="6"/>
+      <c r="AB9" s="8"/>
       <c r="AC9" s="7"/>
+      <c r="AD9" s="8"/>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O10" s="10"/>
+      <c r="P10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" s="10"/>
+      <c r="T10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="U10" s="10"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="B11" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="n">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="I11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5" t="s">
+      <c r="L11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="6" t="s">
+      <c r="R11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="7"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC10"/>
+  <autoFilter ref="A1:AD11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>